<commit_message>
Memo and TODO list update
Updated the memo, TODO list, and Weight List with the information I had.
</commit_message>
<xml_diff>
--- a/Design/Weight List.xlsx
+++ b/Design/Weight List.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="168" windowWidth="14808" windowHeight="7956"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Component</t>
   </si>
@@ -41,6 +41,21 @@
   </si>
   <si>
     <t>Max Weight</t>
+  </si>
+  <si>
+    <t>Chassis</t>
+  </si>
+  <si>
+    <t>Position Feedback Cylinder 1-1/16"</t>
+  </si>
+  <si>
+    <t>Solenoid Valve</t>
+  </si>
+  <si>
+    <t>4/2 DCV</t>
+  </si>
+  <si>
+    <t>Position Feedback Cylinder 2"</t>
   </si>
 </sst>
 </file>
@@ -175,7 +190,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -210,7 +225,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -422,12 +437,12 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -464,6 +479,46 @@
         <v>0.5</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>2.2429999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <v>0.91800000000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>3.6900000000000002E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>0.13</v>
+      </c>
+    </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E19" t="s">
         <v>8</v>
@@ -475,7 +530,7 @@
       </c>
       <c r="B20" s="2">
         <f>SUM(B2:B19)</f>
-        <v>2.8050000000000002</v>
+        <v>6.3329000000000004</v>
       </c>
       <c r="E20">
         <v>35</v>
@@ -487,7 +542,7 @@
       </c>
       <c r="B21">
         <f>B20*1.25</f>
-        <v>3.5062500000000001</v>
+        <v>7.916125000000001</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -496,7 +551,7 @@
       </c>
       <c r="B22" s="3">
         <f>B20+B21</f>
-        <v>6.3112500000000002</v>
+        <v>14.249025000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>